<commit_message>
collapsed observeEvents into a single line - better!
</commit_message>
<xml_diff>
--- a/data/country_defaults.xlsx
+++ b/data/country_defaults.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24519"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30A40DE2-E0FB-4E46-AF3B-DBF405101C45}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD498611-1ABB-4542-9995-ADC5D3018F0F}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>country</t>
   </si>
@@ -46,10 +46,13 @@
     <t>Vietnam</t>
   </si>
   <si>
-    <t>flock_growth</t>
-  </si>
-  <si>
-    <t>flock_mortality</t>
+    <t>growth</t>
+  </si>
+  <si>
+    <t>mortality</t>
+  </si>
+  <si>
+    <t>perc_laying</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -490,6 +493,28 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added all costs - it's overly busy but works
</commit_message>
<xml_diff>
--- a/data/country_defaults.xlsx
+++ b/data/country_defaults.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24519"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49B7DAA3-B6A4-43BD-B85E-DC7BEA4D6D17}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09878AF9-358D-4CD4-8B8D-6381A1C7CB8D}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
   <si>
     <t>country</t>
   </si>
@@ -59,14 +59,55 @@
   </si>
   <si>
     <t>breakage</t>
+  </si>
+  <si>
+    <t>price_egg</t>
+  </si>
+  <si>
+    <t>price_spent</t>
+  </si>
+  <si>
+    <t>price_manure</t>
+  </si>
+  <si>
+    <t>cost_feed</t>
+  </si>
+  <si>
+    <t>cost_labor</t>
+  </si>
+  <si>
+    <t>cost_pullet</t>
+  </si>
+  <si>
+    <t>cost_equip</t>
+  </si>
+  <si>
+    <t>cost_litter</t>
+  </si>
+  <si>
+    <t>cost_vet</t>
+  </si>
+  <si>
+    <t>cost_land</t>
+  </si>
+  <si>
+    <t>cost_office</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -94,9 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -423,13 +465,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -563,6 +605,248 @@
       </c>
       <c r="C13" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35">
+        <v>34000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to add flags to the country list - not successful yet...
</commit_message>
<xml_diff>
--- a/data/country_defaults.xlsx
+++ b/data/country_defaults.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24519"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="104" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09878AF9-358D-4CD4-8B8D-6381A1C7CB8D}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{414022A5-FF51-48D0-A743-23170B27D14E}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="23">
   <si>
     <t>country</t>
   </si>
@@ -40,58 +40,61 @@
     <t>China</t>
   </si>
   <si>
+    <t>breakage</t>
+  </si>
+  <si>
+    <t>cost_equip</t>
+  </si>
+  <si>
+    <t>cost_feed</t>
+  </si>
+  <si>
+    <t>cost_labor</t>
+  </si>
+  <si>
+    <t>cost_land</t>
+  </si>
+  <si>
+    <t>cost_litter</t>
+  </si>
+  <si>
+    <t>cost_office</t>
+  </si>
+  <si>
+    <t>cost_pullet</t>
+  </si>
+  <si>
+    <t>cost_vet</t>
+  </si>
+  <si>
+    <t>eggs_laid</t>
+  </si>
+  <si>
     <t>flock_size</t>
   </si>
   <si>
+    <t>growth</t>
+  </si>
+  <si>
+    <t>mortality</t>
+  </si>
+  <si>
+    <t>perc_laying</t>
+  </si>
+  <si>
+    <t>price_egg</t>
+  </si>
+  <si>
+    <t>price_manure</t>
+  </si>
+  <si>
+    <t>price_spent</t>
+  </si>
+  <si>
     <t>Vietnam</t>
   </si>
   <si>
-    <t>growth</t>
-  </si>
-  <si>
-    <t>mortality</t>
-  </si>
-  <si>
-    <t>perc_laying</t>
-  </si>
-  <si>
-    <t>eggs_laid</t>
-  </si>
-  <si>
-    <t>breakage</t>
-  </si>
-  <si>
-    <t>price_egg</t>
-  </si>
-  <si>
-    <t>price_spent</t>
-  </si>
-  <si>
-    <t>price_manure</t>
-  </si>
-  <si>
-    <t>cost_feed</t>
-  </si>
-  <si>
-    <t>cost_labor</t>
-  </si>
-  <si>
-    <t>cost_pullet</t>
-  </si>
-  <si>
-    <t>cost_equip</t>
-  </si>
-  <si>
-    <t>cost_litter</t>
-  </si>
-  <si>
-    <t>cost_vet</t>
-  </si>
-  <si>
-    <t>cost_land</t>
-  </si>
-  <si>
-    <t>cost_office</t>
+    <t>Cambodia</t>
   </si>
 </sst>
 </file>
@@ -453,14 +456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A1048556" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -482,19 +486,19 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>10000</v>
+      <c r="C2" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3">
-        <v>5000</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -504,19 +508,19 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1">
-        <v>5</v>
+      <c r="C4">
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1.2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -524,21 +528,21 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>30000</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -546,21 +550,21 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1">
-        <v>85</v>
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>34000</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>85</v>
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -568,21 +572,21 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>357</v>
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
-        <v>400</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -590,21 +594,21 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>10000</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1">
         <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1">
-        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -612,10 +616,10 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1">
-        <v>0.53</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -623,10 +627,10 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1">
-        <v>0.21</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -634,222 +638,430 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1">
-        <v>0.11</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1">
-        <v>1.2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1">
-        <v>0.09</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1">
-        <v>0.2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>1000</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C21">
-        <v>1.2</v>
+        <v>800</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>1.1000000000000001</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C26">
-        <v>800</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C27">
-        <v>1.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="C28" s="1">
+        <v>400</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C29">
-        <v>0.4</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30">
-        <v>1.1000000000000001</v>
+        <v>15</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31">
-        <v>0.9</v>
+        <v>16</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
         <v>5</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C37">
+        <v>1.4</v>
+      </c>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>801</v>
+      </c>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <v>2.8</v>
+      </c>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>40001</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>2.1</v>
+      </c>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>50001</v>
+      </c>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44">
+        <v>1.9</v>
+      </c>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="1">
+        <v>401</v>
+      </c>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46">
+        <v>5001</v>
+      </c>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="1">
+        <v>4</v>
+      </c>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="1">
+        <v>86</v>
+      </c>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" t="s">
         <v>20</v>
       </c>
-      <c r="C32">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35">
-        <v>34000</v>
-      </c>
+      <c r="C52" s="1">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D52" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C35">
+    <sortCondition ref="A2:A35"/>
+    <sortCondition ref="B2:B35"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>